<commit_message>
Cleaning needs to be done
</commit_message>
<xml_diff>
--- a/LOTR.xlsx
+++ b/LOTR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blaz/Desktop/LOTR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8C1414-163F-F749-B9D5-A532ACF266C8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C343DFEB-DBE5-A44A-8A4C-8B7312C2951E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="620" windowWidth="22500" windowHeight="15360" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="The Silmarillion" sheetId="1" r:id="rId1"/>
@@ -22,23 +22,12 @@
     <sheet name="Combined" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'The Silmarillion'!$A$2:$A$29</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'The Silmarillion'!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'The Silmarillion'!$B$2:$B$29</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'The Silmarillion'!$A$2:$A$29</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'The Silmarillion'!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'The Silmarillion'!$B$2:$B$29</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'The Silmarillion'!$A$2:$A$29</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'The Silmarillion'!$B$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'The Silmarillion'!$B$2:$B$29</definedName>
-  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="318">
   <si>
     <t>Polarity</t>
   </si>
@@ -439,32 +428,566 @@
     <t>Use topic modeling to take a deeper look at chapters that have a polarity of 0</t>
   </si>
   <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>Hobbit</t>
-  </si>
-  <si>
-    <t>Fellowship</t>
-  </si>
-  <si>
-    <t>Two Towers</t>
-  </si>
-  <si>
-    <t>Simarillion</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Unique words</t>
+    <t>long</t>
+  </si>
+  <si>
+    <t>better</t>
+  </si>
+  <si>
+    <t>door</t>
+  </si>
+  <si>
+    <t>fell</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>began</t>
+  </si>
+  <si>
+    <t>beren</t>
+  </si>
+  <si>
+    <t>suddenly</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>turned</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>saw</t>
+  </si>
+  <si>
+    <t>hills</t>
+  </si>
+  <si>
+    <t>north</t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>tale</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>silent</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>pony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hill </t>
+  </si>
+  <si>
+    <t>think</t>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>stood</t>
+  </si>
+  <si>
+    <t>answered</t>
+  </si>
+  <si>
+    <t>ago</t>
+  </si>
+  <si>
+    <t>shapes</t>
+  </si>
+  <si>
+    <t>shadow</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>far</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>did</t>
+  </si>
+  <si>
+    <t>feet</t>
+  </si>
+  <si>
+    <t>little</t>
+  </si>
+  <si>
+    <t>elves</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">line </t>
+  </si>
+  <si>
+    <t>moment</t>
+  </si>
+  <si>
+    <t>away</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>dark</t>
+  </si>
+  <si>
+    <t>hope</t>
+  </si>
+  <si>
+    <t>hobbits</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>enemy</t>
+  </si>
+  <si>
+    <t>lost</t>
+  </si>
+  <si>
+    <t>cold</t>
+  </si>
+  <si>
+    <t>orcs</t>
+  </si>
+  <si>
+    <t>boat</t>
+  </si>
+  <si>
+    <t>taken</t>
+  </si>
+  <si>
+    <t>river</t>
+  </si>
+  <si>
+    <t>way</t>
+  </si>
+  <si>
+    <t>fallen</t>
+  </si>
+  <si>
+    <t>slain</t>
+  </si>
+  <si>
+    <t>roaring</t>
+  </si>
+  <si>
+    <t>mordor</t>
+  </si>
+  <si>
+    <t>alas</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>lands</t>
+  </si>
+  <si>
+    <t>sprang</t>
+  </si>
+  <si>
+    <t>late</t>
+  </si>
+  <si>
+    <t>wish</t>
+  </si>
+  <si>
+    <t>swift</t>
+  </si>
+  <si>
+    <t>eyes</t>
+  </si>
+  <si>
+    <t>horn</t>
+  </si>
+  <si>
+    <t>laid</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>south</t>
+  </si>
+  <si>
+    <t>arrows</t>
+  </si>
+  <si>
+    <t>dwarves</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>bore</t>
+  </si>
+  <si>
+    <t>saruman</t>
+  </si>
+  <si>
+    <t>swords</t>
+  </si>
+  <si>
+    <t>shore</t>
+  </si>
+  <si>
+    <t>seen</t>
+  </si>
+  <si>
+    <t>wild</t>
+  </si>
+  <si>
+    <t>gondor</t>
+  </si>
+  <si>
+    <t>dread</t>
+  </si>
+  <si>
+    <t>doubt</t>
+  </si>
+  <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>tall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seen </t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>nearer</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>darkness</t>
+  </si>
+  <si>
+    <t>morning</t>
+  </si>
+  <si>
+    <t>stone</t>
+  </si>
+  <si>
+    <t>walls</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>hear</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>leading</t>
+  </si>
+  <si>
+    <t>don</t>
+  </si>
+  <si>
+    <t>woods</t>
+  </si>
+  <si>
+    <t>air</t>
+  </si>
+  <si>
+    <t>east</t>
+  </si>
+  <si>
+    <t>words</t>
+  </si>
+  <si>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>lord</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>ships</t>
+  </si>
+  <si>
+    <t>battle</t>
+  </si>
+  <si>
+    <t>foes</t>
+  </si>
+  <si>
+    <t>face</t>
+  </si>
+  <si>
+    <t>borne</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>wrath</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>bity</t>
+  </si>
+  <si>
+    <t>cried</t>
+  </si>
+  <si>
+    <t>death</t>
+  </si>
+  <si>
+    <t>tears</t>
+  </si>
+  <si>
+    <t>took</t>
+  </si>
+  <si>
+    <t>banner</t>
+  </si>
+  <si>
+    <t>despair</t>
+  </si>
+  <si>
+    <t>fury</t>
+  </si>
+  <si>
+    <t>servants</t>
+  </si>
+  <si>
+    <t>tower</t>
+  </si>
+  <si>
+    <t>lies</t>
+  </si>
+  <si>
+    <t>broke</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>given</t>
+  </si>
+  <si>
+    <t>terrible</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>heart</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>fields</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>army</t>
+  </si>
+  <si>
+    <t>forth</t>
+  </si>
+  <si>
+    <t>mind</t>
+  </si>
+  <si>
+    <t>silenece</t>
+  </si>
+  <si>
+    <t>destroyed</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>assault</t>
+  </si>
+  <si>
+    <t>scouts</t>
+  </si>
+  <si>
+    <t>blew</t>
+  </si>
+  <si>
+    <t>watched</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>sauron</t>
+  </si>
+  <si>
+    <t>lay</t>
+  </si>
+  <si>
+    <t>heralds</t>
+  </si>
+  <si>
+    <t>terms</t>
+  </si>
+  <si>
+    <t>guard</t>
+  </si>
+  <si>
+    <t>war</t>
+  </si>
+  <si>
+    <t>blade</t>
+  </si>
+  <si>
+    <t>rohan</t>
+  </si>
+  <si>
+    <t>eastward</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>miles</t>
+  </si>
+  <si>
+    <t>clouds</t>
+  </si>
+  <si>
+    <t>effort</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>gone</t>
+  </si>
+  <si>
+    <t>thing</t>
+  </si>
+  <si>
+    <t>dreadful</t>
+  </si>
+  <si>
+    <t>burden</t>
+  </si>
+  <si>
+    <t>plain</t>
+  </si>
+  <si>
+    <t>lying</t>
+  </si>
+  <si>
+    <t>worn</t>
+  </si>
+  <si>
+    <t>coming</t>
+  </si>
+  <si>
+    <t>tearing</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>deep</t>
+  </si>
+  <si>
+    <t>just</t>
+  </si>
+  <si>
+    <t>breast</t>
+  </si>
+  <si>
+    <t>muttered</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>things</t>
+  </si>
+  <si>
+    <t>felt</t>
+  </si>
+  <si>
+    <t>slowly</t>
+  </si>
+  <si>
+    <t>head</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14605,13 +15128,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -14619,7 +15142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -14627,7 +15150,7 @@
         <v>1.666666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -14635,7 +15158,7 @@
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -14643,7 +15166,7 @@
         <v>2.8571428571428572</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -14651,7 +15174,7 @@
         <v>2.666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -14659,7 +15182,7 @@
         <v>2.285714285714286</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -14667,7 +15190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -14675,7 +15198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -14683,7 +15206,7 @@
         <v>2.666666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -14691,7 +15214,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -14699,7 +15222,7 @@
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -14707,7 +15230,7 @@
         <v>0.72727272727272729</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -14715,7 +15238,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -14723,7 +15246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -14731,7 +15254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -14739,7 +15262,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -14747,7 +15270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -14755,7 +15278,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -14763,7 +15286,7 @@
         <v>1.714285714285714</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -14771,7 +15294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -14779,7 +15302,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -14787,7 +15310,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -14795,7 +15318,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -14803,7 +15326,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -14811,7 +15334,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -14819,7 +15342,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -14827,7 +15350,7 @@
         <v>1.142857142857143</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -14835,7 +15358,7 @@
         <v>1.84375</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -14857,15 +15380,15 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -14873,7 +15396,7 @@
         <v>2.2666666666666671</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -14881,7 +15404,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -14889,7 +15412,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -14897,7 +15420,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -14905,7 +15428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -14913,7 +15436,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -14921,7 +15444,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -14929,7 +15452,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -14937,7 +15460,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -14945,7 +15468,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -14953,7 +15476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -14961,7 +15484,7 @@
         <v>0.61538461538461542</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -14969,7 +15492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -14977,7 +15500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -14985,7 +15508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -14993,7 +15516,7 @@
         <v>2.666666666666667</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
@@ -15001,7 +15524,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -15009,7 +15532,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -15031,13 +15554,13 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -15045,7 +15568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -15053,7 +15576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -15061,7 +15584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
@@ -15069,7 +15592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -15077,7 +15600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -15085,7 +15608,7 @@
         <v>2.333333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -15093,7 +15616,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -15101,7 +15624,7 @@
         <v>1.1764705882352939</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -15109,7 +15632,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -15117,7 +15640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>59</v>
       </c>
@@ -15125,7 +15648,7 @@
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -15133,7 +15656,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
@@ -15141,7 +15664,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>62</v>
       </c>
@@ -15149,7 +15672,7 @@
         <v>2.3636363636363642</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -15157,7 +15680,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
@@ -15165,7 +15688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -15173,7 +15696,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -15181,7 +15704,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>67</v>
       </c>
@@ -15189,7 +15712,7 @@
         <v>0.89655172413793105</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>68</v>
       </c>
@@ -15197,7 +15720,7 @@
         <v>1.4736842105263159</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>69</v>
       </c>
@@ -15205,7 +15728,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
@@ -15213,7 +15736,7 @@
         <v>0.22222222222222221</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -15221,7 +15744,7 @@
         <v>0.23529411764705879</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -15229,7 +15752,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
@@ -15237,7 +15760,7 @@
         <v>2.545454545454545</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -15245,7 +15768,7 @@
         <v>0.30769230769230771</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>75</v>
       </c>
@@ -15267,9 +15790,9 @@
       <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -15277,7 +15800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
@@ -15285,7 +15808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -15293,7 +15816,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -15301,7 +15824,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -15309,7 +15832,7 @@
         <v>2.347826086956522</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>81</v>
       </c>
@@ -15317,7 +15840,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
@@ -15325,7 +15848,7 @@
         <v>2.4705882352941182</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>83</v>
       </c>
@@ -15333,7 +15856,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>84</v>
       </c>
@@ -15341,7 +15864,7 @@
         <v>1.571428571428571</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>85</v>
       </c>
@@ -15349,7 +15872,7 @@
         <v>0.42857142857142849</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>86</v>
       </c>
@@ -15357,7 +15880,7 @@
         <v>1.882352941176471</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>87</v>
       </c>
@@ -15365,7 +15888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>88</v>
       </c>
@@ -15373,7 +15896,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
@@ -15381,7 +15904,7 @@
         <v>0.61538461538461542</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>90</v>
       </c>
@@ -15389,7 +15912,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -15397,7 +15920,7 @@
         <v>1.833333333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>92</v>
       </c>
@@ -15405,7 +15928,7 @@
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
@@ -15413,7 +15936,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>94</v>
       </c>
@@ -15421,7 +15944,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>95</v>
       </c>
@@ -15429,7 +15952,7 @@
         <v>1.166666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
@@ -15437,7 +15960,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>97</v>
       </c>
@@ -15459,13 +15982,13 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -15473,7 +15996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -15481,7 +16004,7 @@
         <v>1.9130434782608701</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -15489,7 +16012,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
@@ -15497,7 +16020,7 @@
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>102</v>
       </c>
@@ -15505,7 +16028,7 @@
         <v>0.76190476190476186</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>103</v>
       </c>
@@ -15513,7 +16036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>104</v>
       </c>
@@ -15521,7 +16044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -15529,7 +16052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>106</v>
       </c>
@@ -15537,7 +16060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>107</v>
       </c>
@@ -15545,7 +16068,7 @@
         <v>1.7777777777777779</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>108</v>
       </c>
@@ -15553,7 +16076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>109</v>
       </c>
@@ -15561,7 +16084,7 @@
         <v>0.47058823529411759</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>110</v>
       </c>
@@ -15569,7 +16092,7 @@
         <v>0.1333333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>111</v>
       </c>
@@ -15577,7 +16100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>112</v>
       </c>
@@ -15585,7 +16108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>113</v>
       </c>
@@ -15593,7 +16116,7 @@
         <v>2.4615384615384621</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>114</v>
       </c>
@@ -15601,7 +16124,7 @@
         <v>2.307692307692307</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>115</v>
       </c>
@@ -15609,7 +16132,7 @@
         <v>1.428571428571429</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>116</v>
       </c>
@@ -15617,7 +16140,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>117</v>
       </c>
@@ -15639,7 +16162,7 @@
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -15652,7 +16175,7 @@
     <col min="14" max="14" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -15670,7 +16193,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
@@ -15696,7 +16219,7 @@
         <v>1.9130434782608701</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -15722,7 +16245,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -15748,7 +16271,7 @@
         <v>1.333333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -15774,7 +16297,7 @@
         <v>0.76190476190476186</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -15800,7 +16323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -15826,7 +16349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -15852,7 +16375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -15878,7 +16401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
@@ -15904,7 +16427,7 @@
         <v>1.7777777777777779</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -15930,7 +16453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -15956,7 +16479,7 @@
         <v>0.47058823529411759</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -15982,7 +16505,7 @@
         <v>0.1333333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -16008,7 +16531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -16034,7 +16557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -16060,7 +16583,7 @@
         <v>2.4615384615384621</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -16086,7 +16609,7 @@
         <v>2.307692307692307</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
@@ -16112,7 +16635,7 @@
         <v>1.428571428571429</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -16138,7 +16661,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -16164,7 +16687,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
@@ -16178,7 +16701,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E22" s="1" t="s">
         <v>70</v>
       </c>
@@ -16192,7 +16715,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E23" s="1" t="s">
         <v>71</v>
       </c>
@@ -16200,7 +16723,7 @@
         <v>0.23529411764705879</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E24" s="1" t="s">
         <v>72</v>
       </c>
@@ -16208,7 +16731,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E25" s="1" t="s">
         <v>73</v>
       </c>
@@ -16216,7 +16739,7 @@
         <v>2.545454545454545</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E26" s="1" t="s">
         <v>74</v>
       </c>
@@ -16224,7 +16747,7 @@
         <v>0.30769230769230771</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E27" s="1" t="s">
         <v>75</v>
       </c>
@@ -16246,19 +16769,19 @@
       <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -16266,7 +16789,7 @@
         <v>1.6666666699999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -16274,7 +16797,7 @@
         <v>3.3333333299999999</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -16282,7 +16805,7 @@
         <v>2.8571428600000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -16290,7 +16813,7 @@
         <v>2.6666666700000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -16298,7 +16821,7 @@
         <v>2.28571429</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -16306,7 +16829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>121</v>
       </c>
@@ -16314,7 +16837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>122</v>
       </c>
@@ -16322,7 +16845,7 @@
         <v>2.6666666700000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -16330,7 +16853,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -16338,7 +16861,7 @@
         <v>1.3333333300000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -16346,7 +16869,7 @@
         <v>0.72727273000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16">
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -16354,7 +16877,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -16362,7 +16885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -16370,7 +16893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -16378,7 +16901,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -16386,7 +16909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -16394,7 +16917,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16">
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -16402,7 +16925,7 @@
         <v>1.71428571</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -16410,7 +16933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -16418,7 +16941,7 @@
         <v>0.90909090999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16">
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>123</v>
       </c>
@@ -16426,7 +16949,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -16434,7 +16957,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16">
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>124</v>
       </c>
@@ -16442,7 +16965,7 @@
         <v>0.66666667000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -16450,7 +16973,7 @@
         <v>0.66666667000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16">
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -16458,7 +16981,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16">
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>125</v>
       </c>
@@ -16466,7 +16989,7 @@
         <v>1.14285714</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16">
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>126</v>
       </c>
@@ -16474,7 +16997,7 @@
         <v>1.84375</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -16482,7 +17005,7 @@
         <v>1.84375</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16">
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -16490,7 +17013,7 @@
         <v>2.2666666700000002</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -16498,7 +17021,7 @@
         <v>0.44444444</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16">
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -16506,7 +17029,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -16514,7 +17037,7 @@
         <v>0.57142857000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16">
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -16522,7 +17045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -16530,7 +17053,7 @@
         <v>0.66666667000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16">
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -16538,7 +17061,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16">
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -16546,7 +17069,7 @@
         <v>0.33333332999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16">
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -16554,7 +17077,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -16562,7 +17085,7 @@
         <v>0.28571428999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16">
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -16570,7 +17093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16">
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -16578,7 +17101,7 @@
         <v>0.61538462000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16">
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -16586,7 +17109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16">
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -16594,7 +17117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16">
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -16602,7 +17125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="16">
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
@@ -16610,7 +17133,7 @@
         <v>2.6666666700000001</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16">
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -16618,7 +17141,7 @@
         <v>0.57142857000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16">
+    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
@@ -16626,7 +17149,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16">
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>48</v>
       </c>
@@ -16634,7 +17157,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16">
+    <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>50</v>
       </c>
@@ -16642,7 +17165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16">
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -16650,7 +17173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16">
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>52</v>
       </c>
@@ -16658,7 +17181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16">
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -16666,7 +17189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16">
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
@@ -16674,7 +17197,7 @@
         <v>2.3333333299999999</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16">
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
@@ -16682,7 +17205,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16">
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>56</v>
       </c>
@@ -16690,7 +17213,7 @@
         <v>1.1764705900000001</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16">
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
@@ -16698,7 +17221,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16">
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
@@ -16706,7 +17229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16">
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
@@ -16714,7 +17237,7 @@
         <v>1.3333333300000001</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16">
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
@@ -16722,7 +17245,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16">
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
@@ -16730,7 +17253,7 @@
         <v>0.66666667000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16">
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
@@ -16738,7 +17261,7 @@
         <v>2.3636363600000001</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16">
+    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>63</v>
       </c>
@@ -16746,7 +17269,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16">
+    <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
@@ -16754,7 +17277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16">
+    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>65</v>
       </c>
@@ -16762,7 +17285,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="16">
+    <row r="65" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
@@ -16770,7 +17293,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="16">
+    <row r="66" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>67</v>
       </c>
@@ -16778,7 +17301,7 @@
         <v>0.89655172000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="16">
+    <row r="67" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
@@ -16786,7 +17309,7 @@
         <v>1.47368421</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="16">
+    <row r="68" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>69</v>
       </c>
@@ -16794,7 +17317,7 @@
         <v>0.28571428999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="16">
+    <row r="69" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>127</v>
       </c>
@@ -16802,7 +17325,7 @@
         <v>0.22222222</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="16">
+    <row r="70" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>128</v>
       </c>
@@ -16810,7 +17333,7 @@
         <v>0.23529412</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="16">
+    <row r="71" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>72</v>
       </c>
@@ -16821,7 +17344,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="16">
+    <row r="72" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>129</v>
       </c>
@@ -16829,7 +17352,7 @@
         <v>2.5454545500000001</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="16">
+    <row r="73" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>74</v>
       </c>
@@ -16837,7 +17360,7 @@
         <v>0.30769231000000002</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="16">
+    <row r="74" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>75</v>
       </c>
@@ -16845,7 +17368,7 @@
         <v>0.18181818</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="16">
+    <row r="75" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>77</v>
       </c>
@@ -16853,7 +17376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="16">
+    <row r="76" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
@@ -16861,7 +17384,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="16">
+    <row r="77" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>79</v>
       </c>
@@ -16869,7 +17392,7 @@
         <v>0.85714285999999995</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="16">
+    <row r="78" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>80</v>
       </c>
@@ -16877,7 +17400,7 @@
         <v>2.3478260899999999</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="16">
+    <row r="79" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>81</v>
       </c>
@@ -16885,7 +17408,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="16">
+    <row r="80" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>82</v>
       </c>
@@ -16893,7 +17416,7 @@
         <v>2.4705882400000001</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="16">
+    <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>83</v>
       </c>
@@ -16901,7 +17424,7 @@
         <v>0.57142857000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16">
+    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>84</v>
       </c>
@@ -16909,7 +17432,7 @@
         <v>1.5714285699999999</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16">
+    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>85</v>
       </c>
@@ -16917,7 +17440,7 @@
         <v>0.42857142999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16">
+    <row r="84" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>86</v>
       </c>
@@ -16925,7 +17448,7 @@
         <v>1.8823529400000001</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16">
+    <row r="85" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>130</v>
       </c>
@@ -16933,7 +17456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16">
+    <row r="86" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>88</v>
       </c>
@@ -16941,7 +17464,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16">
+    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>89</v>
       </c>
@@ -16949,7 +17472,7 @@
         <v>0.61538462000000005</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16">
+    <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>90</v>
       </c>
@@ -16957,7 +17480,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16">
+    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>91</v>
       </c>
@@ -16965,7 +17488,7 @@
         <v>1.8333333300000001</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="16">
+    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>92</v>
       </c>
@@ -16973,7 +17496,7 @@
         <v>1.3333333300000001</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16">
+    <row r="91" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>93</v>
       </c>
@@ -16981,7 +17504,7 @@
         <v>0.88888889000000004</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16">
+    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>94</v>
       </c>
@@ -16989,7 +17512,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="16">
+    <row r="93" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>95</v>
       </c>
@@ -16997,7 +17520,7 @@
         <v>1.1666666699999999</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="16">
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>96</v>
       </c>
@@ -17005,7 +17528,7 @@
         <v>0.44444444</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="16">
+    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>97</v>
       </c>
@@ -17013,7 +17536,7 @@
         <v>0.85714285999999995</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="16">
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>99</v>
       </c>
@@ -17021,7 +17544,7 @@
         <v>1.91304348</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="16">
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
@@ -17029,7 +17552,7 @@
         <v>0.66666667000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="16">
+    <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
@@ -17037,7 +17560,7 @@
         <v>1.3333333300000001</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="16">
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>102</v>
       </c>
@@ -17045,7 +17568,7 @@
         <v>0.76190475999999996</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="16">
+    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>103</v>
       </c>
@@ -17053,7 +17576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16">
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
@@ -17061,7 +17584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="16">
+    <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>105</v>
       </c>
@@ -17069,7 +17592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="16">
+    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
@@ -17077,7 +17600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="16">
+    <row r="104" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>107</v>
       </c>
@@ -17085,7 +17608,7 @@
         <v>1.7777777800000001</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="16">
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>108</v>
       </c>
@@ -17093,7 +17616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="16">
+    <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>109</v>
       </c>
@@ -17101,7 +17624,7 @@
         <v>0.47058823999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="16">
+    <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>110</v>
       </c>
@@ -17109,7 +17632,7 @@
         <v>0.13333333</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="16">
+    <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>111</v>
       </c>
@@ -17117,7 +17640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="16">
+    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>112</v>
       </c>
@@ -17125,7 +17648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="16">
+    <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>113</v>
       </c>
@@ -17133,7 +17656,7 @@
         <v>2.4615384599999999</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="16">
+    <row r="111" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>114</v>
       </c>
@@ -17141,7 +17664,7 @@
         <v>2.3076923100000002</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="16">
+    <row r="112" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>115</v>
       </c>
@@ -17149,7 +17672,7 @@
         <v>1.4285714300000001</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="16">
+    <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>116</v>
       </c>
@@ -17157,7 +17680,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="16">
+    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>117</v>
       </c>
@@ -17165,7 +17688,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F126" t="s">
         <v>132</v>
       </c>
@@ -17179,82 +17702,1401 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F86FE1A-7D86-F146-A17C-E80434683304}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>133</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>138</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="3">
-        <v>148914</v>
-      </c>
-      <c r="C2" s="3">
-        <v>7145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="3">
-        <v>96180</v>
-      </c>
-      <c r="C3" s="3">
-        <v>6187</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="3">
-        <v>182858</v>
-      </c>
-      <c r="C4" s="3">
-        <v>8528</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="3">
-        <v>155947</v>
-      </c>
-      <c r="C5" s="3">
-        <v>7758</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="3">
-        <v>132059</v>
-      </c>
-      <c r="C6" s="3">
-        <v>7008</v>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>